<commit_message>
Bugfix sur la masse des LEDs. Recompile OK. Ajout des outputjobs demandes
</commit_message>
<xml_diff>
--- a/Project Outputs for TP2/BOM/Bill of Materials-Bill of Materials.xlsx
+++ b/Project Outputs for TP2/BOM/Bill of Materials-Bill of Materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22860" windowHeight="15465"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21390" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Bill of Mater" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
   <si>
     <t>Comment</t>
   </si>
@@ -69,7 +69,7 @@
     <t/>
   </si>
   <si>
-    <t>RAD-0.3</t>
+    <t>CAPC1608N</t>
   </si>
   <si>
     <t>C1, C2, C3, C4, C5, C6, C15</t>
@@ -87,6 +87,9 @@
     <t>[NoValue], TDK, TDK, TDK</t>
   </si>
   <si>
+    <t>CAPC2012N</t>
+  </si>
+  <si>
     <t>[NoValue], Farnell, Farnell, Farnell</t>
   </si>
   <si>
@@ -105,6 +108,33 @@
     <t>C10, C14</t>
   </si>
   <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>Typical RED, GREEN, YELLOW, AMBER GaAs LED</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>KINGBRIGHT</t>
+  </si>
+  <si>
+    <t>LED 0805</t>
+  </si>
+  <si>
+    <t>Farnell</t>
+  </si>
+  <si>
+    <t>KPT-2012SGC</t>
+  </si>
+  <si>
+    <t>2099239</t>
+  </si>
+  <si>
+    <t>D1_LED0, D1_LED1, D1_LED2, D1_LED3, D4</t>
+  </si>
+  <si>
     <t>GF1A</t>
   </si>
   <si>
@@ -117,10 +147,7 @@
     <t>VISHAY</t>
   </si>
   <si>
-    <t>SMC</t>
-  </si>
-  <si>
-    <t>Farnell</t>
+    <t>SMA/DO-214AC_21</t>
   </si>
   <si>
     <t>GF1A-E3/67A</t>
@@ -132,30 +159,6 @@
     <t>D2, D3</t>
   </si>
   <si>
-    <t>Green LED</t>
-  </si>
-  <si>
-    <t>Typical RED, GREEN, YELLOW, AMBER GaAs LED</t>
-  </si>
-  <si>
-    <t>LED2</t>
-  </si>
-  <si>
-    <t>KINGBRIGHT</t>
-  </si>
-  <si>
-    <t>3.2X1.6X1.1</t>
-  </si>
-  <si>
-    <t>KPT-2012SGC</t>
-  </si>
-  <si>
-    <t>2099239</t>
-  </si>
-  <si>
-    <t>D4, D4_LED0, D4_LED2, D4_LED11, D4_LED12</t>
-  </si>
-  <si>
     <t>600r</t>
   </si>
   <si>
@@ -165,7 +168,7 @@
     <t>Wurth</t>
   </si>
   <si>
-    <t>INDC1608L</t>
+    <t>INDC1608AN</t>
   </si>
   <si>
     <t>742792651</t>
@@ -183,7 +186,7 @@
     <t>Molex</t>
   </si>
   <si>
-    <t>HDR1X6H</t>
+    <t>RJ12_90</t>
   </si>
   <si>
     <t>53398-0671</t>
@@ -207,7 +210,7 @@
     <t>PHOENIX CONTACT</t>
   </si>
   <si>
-    <t>HDR1X2</t>
+    <t>PHOENIX_1985195</t>
   </si>
   <si>
     <t>PTSA1.5/2-3.5-Z</t>
@@ -228,49 +231,55 @@
     <t>P2</t>
   </si>
   <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>RPot</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>PDB181-K415K-102A2</t>
+  </si>
+  <si>
+    <t>'PDB181-K415K-102A2</t>
+  </si>
+  <si>
+    <t>'1823540</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>330r</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>Res1</t>
+  </si>
+  <si>
     <t>1K</t>
   </si>
   <si>
-    <t>Potentiometer</t>
-  </si>
-  <si>
-    <t>RPot</t>
-  </si>
-  <si>
-    <t>BOURNS</t>
-  </si>
-  <si>
-    <t>VR5</t>
-  </si>
-  <si>
-    <t>PDB181-K415K-102A2</t>
-  </si>
-  <si>
-    <t>1823540</t>
-  </si>
-  <si>
-    <t>R1</t>
+    <t>RESC1608N</t>
+  </si>
+  <si>
+    <t>R2_LED0, R2_LED1, R2_LED2, R2_LED3</t>
   </si>
   <si>
     <t>4.7k</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>Res1</t>
-  </si>
-  <si>
-    <t>AXIAL-0.3</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>330r</t>
-  </si>
-  <si>
-    <t>R2_LED0, R2_LED2, R2_LED11, R2_LED12</t>
+    <t>R3</t>
   </si>
   <si>
     <t>470r</t>
@@ -285,6 +294,9 @@
     <t>Microchip</t>
   </si>
   <si>
+    <t>QFP50P1200X1200X120-64</t>
+  </si>
+  <si>
     <t>1971889</t>
   </si>
   <si>
@@ -297,7 +309,7 @@
     <t>DIODES INC</t>
   </si>
   <si>
-    <t>D2PAK_M</t>
+    <t>TD03B_N</t>
   </si>
   <si>
     <t>AP1117D33G-13</t>
@@ -321,7 +333,7 @@
     <t>FOX ELECTRONICS</t>
   </si>
   <si>
-    <t>R38</t>
+    <t>HC49/4H SMX CRYSTAL</t>
   </si>
   <si>
     <t>FOXSDLF/080-20</t>
@@ -819,24 +831,24 @@
         <v>21</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
@@ -866,123 +878,123 @@
         <v>15</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
@@ -991,33 +1003,33 @@
         <v>15</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
@@ -1026,33 +1038,33 @@
         <v>15</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
@@ -1061,80 +1073,80 @@
         <v>15</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D13" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>15</v>
@@ -1146,30 +1158,30 @@
         <v>15</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="3">
-        <v>4</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="F14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>15</v>
@@ -1181,30 +1193,30 @@
         <v>15</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>15</v>
@@ -1216,18 +1228,18 @@
         <v>15</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D16" s="3">
         <v>1</v>
@@ -1236,33 +1248,33 @@
         <v>15</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D17" s="3">
         <v>1</v>
@@ -1271,33 +1283,33 @@
         <v>15</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D18" s="3">
         <v>1</v>
@@ -1306,22 +1318,22 @@
         <v>15</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>